<commit_message>
Aggiunto gli articoli (WIP)
</commit_message>
<xml_diff>
--- a/venduto 2024.xlsx
+++ b/venduto 2024.xlsx
@@ -8,19 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Edoardo\Documents\fatturazione\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5685A28E-24AD-43D8-A836-944D0FC32729}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86F942B6-7539-48C2-B98F-81E3DB3B9661}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GENNAIO 2024" sheetId="47" r:id="rId1"/>
-    <sheet name="Foglio1" sheetId="53" r:id="rId2"/>
-    <sheet name="Foglio4" sheetId="51" r:id="rId3"/>
-    <sheet name="Testata" sheetId="49" r:id="rId4"/>
-    <sheet name="Corpo" sheetId="48" r:id="rId5"/>
-    <sheet name="Corpo (2)" sheetId="50" r:id="rId6"/>
-    <sheet name="Puntivendita" sheetId="52" r:id="rId7"/>
-    <sheet name="Formati" sheetId="54" r:id="rId8"/>
+    <sheet name="Testata" sheetId="49" r:id="rId2"/>
+    <sheet name="Corpo" sheetId="48" r:id="rId3"/>
+    <sheet name="Corpo (2)" sheetId="50" r:id="rId4"/>
+    <sheet name="Puntivendita" sheetId="52" r:id="rId5"/>
+    <sheet name="Formati" sheetId="54" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'GENNAIO 2024'!$A$1:$AB$156</definedName>
@@ -66,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="433" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="189">
   <si>
     <t>n. buono</t>
   </si>
@@ -209,9 +207,6 @@
     <t>D'AMICIS</t>
   </si>
   <si>
-    <t>008 cav. Int</t>
-  </si>
-  <si>
     <t>MEGAGEST MEGA MARTINA F</t>
   </si>
   <si>
@@ -231,9 +226,6 @@
   </si>
   <si>
     <t>EMMEDUE</t>
-  </si>
-  <si>
-    <t>124     FUSILLI</t>
   </si>
   <si>
     <t xml:space="preserve"> </t>
@@ -428,48 +420,6 @@
     <t>col lunghezza</t>
   </si>
   <si>
-    <t>007  MAR.INT</t>
-  </si>
-  <si>
-    <t>027 ORECCHIETTE_C.RAPA</t>
-  </si>
-  <si>
-    <t>005  OREC_INT</t>
-  </si>
-  <si>
-    <t>006 MACC_INT</t>
-  </si>
-  <si>
-    <t>030   ORECCHIETTE_SECCHE</t>
-  </si>
-  <si>
-    <t>032   CAVATELLI_SECCHE</t>
-  </si>
-  <si>
-    <t>034   TROCCOLI_SECCHE</t>
-  </si>
-  <si>
-    <t>035 PAPP_SEMOLA_SECCHE</t>
-  </si>
-  <si>
-    <t>036 TAGLIATELLE_SEMOLA_SECCHE</t>
-  </si>
-  <si>
-    <t>39 MARITATI_INT_SECCHE</t>
-  </si>
-  <si>
-    <t>042   PAPP_UOVO_SECCHE</t>
-  </si>
-  <si>
-    <t>04 orecch.int_SECCHE</t>
-  </si>
-  <si>
-    <t>0026 ORECCHIETTE_ARSO_SECCHE</t>
-  </si>
-  <si>
-    <t>125     FUSILLI_INT</t>
-  </si>
-  <si>
     <t>0027 ORECCHIETTE C.RAPA</t>
   </si>
   <si>
@@ -560,19 +510,10 @@
     <t xml:space="preserve"> 8032894741051</t>
   </si>
   <si>
-    <t xml:space="preserve">ORECCHIETTE FRESCHE INTEGRALI </t>
-  </si>
-  <si>
     <t xml:space="preserve"> 8032894741068</t>
   </si>
   <si>
-    <t xml:space="preserve">MACCHERONI FRESCHI INTEGRALI </t>
-  </si>
-  <si>
     <t xml:space="preserve"> 8032894741075</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MARITATI FRESCHI INTEGRALI </t>
   </si>
   <si>
     <t xml:space="preserve"> 8032894741099</t>
@@ -611,9 +552,6 @@
     <t>grammi</t>
   </si>
   <si>
-    <t>lprezzo</t>
-  </si>
-  <si>
     <t>sconto</t>
   </si>
   <si>
@@ -627,9 +565,6 @@
   </si>
   <si>
     <t>0032</t>
-  </si>
-  <si>
-    <t>039</t>
   </si>
   <si>
     <t>0101</t>
@@ -681,6 +616,21 @@
   </si>
   <si>
     <t>FUSILLI FRESCHI INTEGRALI</t>
+  </si>
+  <si>
+    <t>0039</t>
+  </si>
+  <si>
+    <t>prezzo</t>
+  </si>
+  <si>
+    <t>ORECCHIETTE FRESCHE INTEGRALI</t>
+  </si>
+  <si>
+    <t>MACCHERONI FRESCHI INTEGRALI</t>
+  </si>
+  <si>
+    <t>MARITATI FRESCHI INTEGRALI</t>
   </si>
 </sst>
 </file>
@@ -1140,7 +1090,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="160">
+  <cellXfs count="161">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1566,12 +1516,7 @@
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="14" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1581,6 +1526,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="21" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="21" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Migliaia" xfId="1" builtinId="3"/>
@@ -1663,7 +1614,7 @@
     <tableColumn id="1" xr3:uid="{73FFD1E5-2614-4127-B002-94701FD92722}" name="ean" dataDxfId="4"/>
     <tableColumn id="3" xr3:uid="{1E2FCAEB-019D-4AA0-BD7F-8D5C7B1BF089}" name="articolo"/>
     <tableColumn id="4" xr3:uid="{D2FBDD2A-F140-416C-AAAF-2085E1B78CF9}" name="grammi" dataDxfId="3"/>
-    <tableColumn id="5" xr3:uid="{E3638016-56B9-4565-9234-D2AA413C5951}" name="lprezzo" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{E3638016-56B9-4565-9234-D2AA413C5951}" name="prezzo" dataDxfId="2"/>
     <tableColumn id="6" xr3:uid="{6A5113FD-B9B8-48DC-BF45-C93B806CC44A}" name="sconto" dataDxfId="1"/>
     <tableColumn id="7" xr3:uid="{68BF6AF6-36C5-4EED-A235-162D48752F0E}" name="iva" dataDxfId="0"/>
   </tableColumns>
@@ -1936,9 +1887,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{168708C7-F2E4-411C-A140-48A329066637}">
   <dimension ref="A1:AF1106"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q5" sqref="Q5"/>
+      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1975,73 +1926,73 @@
         <v>2</v>
       </c>
       <c r="D1" s="55" t="s">
-        <v>144</v>
+        <v>128</v>
       </c>
       <c r="E1" s="56" t="s">
-        <v>145</v>
+        <v>129</v>
       </c>
       <c r="F1" s="57" t="s">
-        <v>146</v>
+        <v>130</v>
       </c>
       <c r="G1" s="58" t="s">
-        <v>147</v>
+        <v>131</v>
       </c>
       <c r="H1" s="59" t="s">
-        <v>148</v>
+        <v>132</v>
       </c>
       <c r="I1" s="60" t="s">
-        <v>149</v>
+        <v>133</v>
       </c>
       <c r="J1" s="65" t="s">
-        <v>150</v>
+        <v>134</v>
       </c>
       <c r="K1" s="100" t="s">
-        <v>151</v>
+        <v>135</v>
       </c>
       <c r="L1" s="61" t="s">
-        <v>152</v>
+        <v>136</v>
       </c>
       <c r="M1" s="62" t="s">
-        <v>153</v>
+        <v>137</v>
       </c>
       <c r="N1" s="63" t="s">
-        <v>154</v>
+        <v>138</v>
       </c>
       <c r="O1" s="95" t="s">
-        <v>134</v>
+        <v>118</v>
       </c>
       <c r="P1" s="64" t="s">
-        <v>135</v>
+        <v>119</v>
       </c>
       <c r="Q1" s="64" t="s">
-        <v>136</v>
+        <v>120</v>
       </c>
       <c r="R1" s="64" t="s">
-        <v>137</v>
+        <v>121</v>
       </c>
       <c r="S1" s="64" t="s">
-        <v>138</v>
+        <v>122</v>
       </c>
       <c r="T1" s="64" t="s">
-        <v>139</v>
+        <v>123</v>
       </c>
       <c r="U1" s="64" t="s">
-        <v>140</v>
+        <v>124</v>
       </c>
       <c r="V1" s="64" t="s">
-        <v>141</v>
+        <v>125</v>
       </c>
       <c r="W1" s="64" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="X1" s="64" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="Y1" s="64" t="s">
-        <v>142</v>
+        <v>126</v>
       </c>
       <c r="Z1" s="64" t="s">
-        <v>143</v>
+        <v>127</v>
       </c>
       <c r="AA1" s="4" t="s">
         <v>32</v>
@@ -2059,7 +2010,7 @@
         <v>45293</v>
       </c>
       <c r="C2" s="82" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D2" s="9">
         <v>15</v>
@@ -2483,7 +2434,7 @@
         <v>45293</v>
       </c>
       <c r="C10" s="91" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D10" s="9">
         <v>25</v>
@@ -2693,7 +2644,7 @@
     </row>
     <row r="14" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A14" s="108" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B14" s="7">
         <v>45295</v>
@@ -2747,7 +2698,7 @@
         <v>45295</v>
       </c>
       <c r="C15" s="91" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D15" s="9"/>
       <c r="E15" s="48"/>
@@ -3001,7 +2952,7 @@
         <v>45296</v>
       </c>
       <c r="C20" s="91" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D20" s="9">
         <v>60</v>
@@ -3172,7 +3123,7 @@
         <v>45296</v>
       </c>
       <c r="C23" s="19" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D23" s="9"/>
       <c r="E23" s="48"/>
@@ -3264,7 +3215,7 @@
         <v>45300</v>
       </c>
       <c r="C25" s="82" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D25" s="9">
         <v>30</v>
@@ -3529,7 +3480,7 @@
         <v>45300</v>
       </c>
       <c r="C30" s="91" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D30" s="9"/>
       <c r="E30" s="48"/>
@@ -4055,7 +4006,7 @@
         <v>45302</v>
       </c>
       <c r="C40" s="91" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D40" s="9">
         <v>40</v>
@@ -4163,7 +4114,7 @@
         <v>45303</v>
       </c>
       <c r="C42" s="82" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D42" s="9">
         <v>30</v>
@@ -4532,7 +4483,7 @@
         <v>45307</v>
       </c>
       <c r="C49" s="91" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D49" s="9">
         <v>25</v>
@@ -4907,7 +4858,7 @@
         <v>45307</v>
       </c>
       <c r="C56" s="107" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D56" s="9">
         <v>40</v>
@@ -5070,7 +5021,7 @@
         <v>45308</v>
       </c>
       <c r="C59" s="81" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D59" s="9">
         <v>9</v>
@@ -5119,7 +5070,7 @@
         <v>45309</v>
       </c>
       <c r="C60" s="91" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D60" s="9">
         <v>40</v>
@@ -5406,7 +5357,7 @@
         <v>45310</v>
       </c>
       <c r="C65" s="91" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D65" s="9">
         <v>40</v>
@@ -5787,7 +5738,7 @@
         <v>45314</v>
       </c>
       <c r="C72" s="91" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D72" s="9">
         <v>30</v>
@@ -6123,7 +6074,7 @@
         <v>45314</v>
       </c>
       <c r="C78" s="107" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D78" s="9"/>
       <c r="E78" s="48"/>
@@ -6470,7 +6421,7 @@
         <v>45316</v>
       </c>
       <c r="C85" s="107" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D85" s="9">
         <v>20</v>
@@ -6629,7 +6580,7 @@
         <v>45317</v>
       </c>
       <c r="C88" s="107" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D88" s="9">
         <v>38</v>
@@ -6794,7 +6745,7 @@
         <v>45317</v>
       </c>
       <c r="C91" s="82" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D91" s="9"/>
       <c r="E91" s="48"/>
@@ -7016,7 +6967,7 @@
         <v>45318</v>
       </c>
       <c r="C95" s="82" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D95" s="9">
         <v>70</v>
@@ -7660,7 +7611,7 @@
         <v>45298</v>
       </c>
       <c r="C107" s="82" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D107" s="9">
         <v>50</v>
@@ -7715,7 +7666,7 @@
         <v>45308</v>
       </c>
       <c r="C108" s="82" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D108" s="9">
         <v>60</v>
@@ -9612,7 +9563,7 @@
       <c r="A159" s="26"/>
       <c r="B159" s="27"/>
       <c r="C159" s="8" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D159" s="28">
         <f t="shared" ref="D159:AB159" si="9">SUM(D2:D158)</f>
@@ -9808,7 +9759,7 @@
       <c r="A162" s="36">
         <v>1</v>
       </c>
-      <c r="B162" s="157" t="s">
+      <c r="B162" s="154" t="s">
         <v>37</v>
       </c>
       <c r="C162" s="83" t="s">
@@ -9924,7 +9875,7 @@
       <c r="A163" s="36">
         <v>2</v>
       </c>
-      <c r="B163" s="157"/>
+      <c r="B163" s="154"/>
       <c r="C163" s="83" t="s">
         <v>24</v>
       </c>
@@ -10037,7 +9988,7 @@
       <c r="A164" s="36">
         <v>3</v>
       </c>
-      <c r="B164" s="157"/>
+      <c r="B164" s="154"/>
       <c r="C164" s="83" t="s">
         <v>25</v>
       </c>
@@ -10150,7 +10101,7 @@
       <c r="A165" s="36">
         <v>4</v>
       </c>
-      <c r="B165" s="157"/>
+      <c r="B165" s="154"/>
       <c r="C165" s="83" t="s">
         <v>27</v>
       </c>
@@ -10263,7 +10214,7 @@
       <c r="A166" s="36">
         <v>5</v>
       </c>
-      <c r="B166" s="157"/>
+      <c r="B166" s="154"/>
       <c r="C166" s="83" t="s">
         <v>41</v>
       </c>
@@ -10376,7 +10327,7 @@
       <c r="A167" s="36">
         <v>6</v>
       </c>
-      <c r="B167" s="157"/>
+      <c r="B167" s="154"/>
       <c r="C167" s="83" t="s">
         <v>14</v>
       </c>
@@ -10489,7 +10440,7 @@
       <c r="A168" s="36">
         <v>7</v>
       </c>
-      <c r="B168" s="157"/>
+      <c r="B168" s="154"/>
       <c r="C168" s="83" t="s">
         <v>29</v>
       </c>
@@ -10602,7 +10553,7 @@
       <c r="A169" s="36">
         <v>8</v>
       </c>
-      <c r="B169" s="157"/>
+      <c r="B169" s="154"/>
       <c r="C169" s="83" t="s">
         <v>31</v>
       </c>
@@ -10715,7 +10666,7 @@
       <c r="A170" s="36">
         <v>9</v>
       </c>
-      <c r="B170" s="157"/>
+      <c r="B170" s="154"/>
       <c r="C170" s="83" t="s">
         <v>20</v>
       </c>
@@ -10828,7 +10779,7 @@
       <c r="A171" s="36">
         <v>10</v>
       </c>
-      <c r="B171" s="157"/>
+      <c r="B171" s="154"/>
       <c r="C171" s="83" t="s">
         <v>15</v>
       </c>
@@ -10941,7 +10892,7 @@
       <c r="A172" s="36">
         <v>11</v>
       </c>
-      <c r="B172" s="157"/>
+      <c r="B172" s="154"/>
       <c r="C172" s="83" t="s">
         <v>18</v>
       </c>
@@ -11054,7 +11005,7 @@
       <c r="A173" s="36">
         <v>12</v>
       </c>
-      <c r="B173" s="157"/>
+      <c r="B173" s="154"/>
       <c r="C173" s="83" t="s">
         <v>13</v>
       </c>
@@ -11167,7 +11118,7 @@
       <c r="A174" s="36">
         <v>13</v>
       </c>
-      <c r="B174" s="157"/>
+      <c r="B174" s="154"/>
       <c r="C174" s="84" t="s">
         <v>23</v>
       </c>
@@ -11280,7 +11231,7 @@
       <c r="A175" s="36">
         <v>14</v>
       </c>
-      <c r="B175" s="157"/>
+      <c r="B175" s="154"/>
       <c r="C175" s="85" t="s">
         <v>28</v>
       </c>
@@ -11393,7 +11344,7 @@
       <c r="A176" s="36">
         <v>15</v>
       </c>
-      <c r="B176" s="157"/>
+      <c r="B176" s="154"/>
       <c r="C176" s="84" t="s">
         <v>26</v>
       </c>
@@ -11506,7 +11457,7 @@
       <c r="A177" s="36">
         <v>16</v>
       </c>
-      <c r="B177" s="157"/>
+      <c r="B177" s="154"/>
       <c r="C177" s="83" t="s">
         <v>17</v>
       </c>
@@ -11619,7 +11570,7 @@
       <c r="A178" s="36">
         <v>17</v>
       </c>
-      <c r="B178" s="157"/>
+      <c r="B178" s="154"/>
       <c r="C178" s="83" t="s">
         <v>16</v>
       </c>
@@ -11732,9 +11683,9 @@
       <c r="A179" s="36">
         <v>18</v>
       </c>
-      <c r="B179" s="157"/>
+      <c r="B179" s="154"/>
       <c r="C179" s="84" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D179" s="40">
         <f t="shared" si="15"/>
@@ -11845,9 +11796,9 @@
       <c r="A180" s="36">
         <v>19</v>
       </c>
-      <c r="B180" s="157"/>
+      <c r="B180" s="154"/>
       <c r="C180" s="84" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D180" s="40">
         <f t="shared" si="15"/>
@@ -11958,9 +11909,9 @@
       <c r="A181" s="36">
         <v>20</v>
       </c>
-      <c r="B181" s="157"/>
+      <c r="B181" s="154"/>
       <c r="C181" s="83" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D181" s="40">
         <f t="shared" si="15"/>
@@ -12071,9 +12022,9 @@
       <c r="A182" s="130">
         <v>21</v>
       </c>
-      <c r="B182" s="158"/>
+      <c r="B182" s="155"/>
       <c r="C182" s="131" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D182" s="132">
         <f t="shared" si="15"/>
@@ -12303,7 +12254,7 @@
       </c>
       <c r="B184" s="47"/>
       <c r="C184" s="82" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D184" s="40">
         <f t="shared" si="17"/>
@@ -12981,7 +12932,7 @@
       </c>
       <c r="B190" s="69"/>
       <c r="C190" s="81" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D190" s="40">
         <f t="shared" ref="D190:N193" si="20">SUMIF($C$2:$C$168,$C190&amp;"*",D$2:D$168)</f>
@@ -13094,7 +13045,7 @@
       </c>
       <c r="B191" s="69"/>
       <c r="C191" s="81" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D191" s="40">
         <f t="shared" si="20"/>
@@ -13207,7 +13158,7 @@
       </c>
       <c r="B192" s="69"/>
       <c r="C192" s="81" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D192" s="40">
         <f t="shared" si="20"/>
@@ -13320,7 +13271,7 @@
       </c>
       <c r="B193" s="69"/>
       <c r="C193" s="81" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D193" s="40">
         <f t="shared" si="20"/>
@@ -13563,7 +13514,7 @@
       <c r="M196" s="24"/>
       <c r="N196" s="24"/>
       <c r="AB196" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="197" spans="1:32" x14ac:dyDescent="0.25">
@@ -36243,465 +36194,6 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF3ED5FE-53C9-4619-BBB0-8414E2FA90CA}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F19F4D68-562A-47BC-8898-153C588B8A33}">
-  <dimension ref="A1:W31"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="22.7109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:23" ht="56.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="55" t="s">
-        <v>3</v>
-      </c>
-      <c r="B1" s="56" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" s="57" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" s="58" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" s="59" t="s">
-        <v>122</v>
-      </c>
-      <c r="F1" s="60" t="s">
-        <v>123</v>
-      </c>
-      <c r="G1" s="65" t="s">
-        <v>120</v>
-      </c>
-      <c r="H1" s="100" t="s">
-        <v>47</v>
-      </c>
-      <c r="I1" s="61" t="s">
-        <v>10</v>
-      </c>
-      <c r="J1" s="62" t="s">
-        <v>11</v>
-      </c>
-      <c r="K1" s="63" t="s">
-        <v>12</v>
-      </c>
-      <c r="L1" s="95" t="s">
-        <v>121</v>
-      </c>
-      <c r="M1" s="64" t="s">
-        <v>124</v>
-      </c>
-      <c r="N1" s="64" t="s">
-        <v>125</v>
-      </c>
-      <c r="O1" s="64" t="s">
-        <v>126</v>
-      </c>
-      <c r="P1" s="64" t="s">
-        <v>127</v>
-      </c>
-      <c r="Q1" s="64" t="s">
-        <v>128</v>
-      </c>
-      <c r="R1" s="64" t="s">
-        <v>129</v>
-      </c>
-      <c r="S1" s="64" t="s">
-        <v>130</v>
-      </c>
-      <c r="T1" s="64" t="s">
-        <v>131</v>
-      </c>
-      <c r="U1" s="64" t="s">
-        <v>132</v>
-      </c>
-      <c r="V1" s="64" t="s">
-        <v>55</v>
-      </c>
-      <c r="W1" s="64" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A3" t="str" cm="1">
-        <f t="array" ref="A3:C3">_xlfn.TEXTSPLIT(A$1," ")</f>
-        <v>001</v>
-      </c>
-      <c r="B3" t="str">
-        <v/>
-      </c>
-      <c r="C3" t="str">
-        <v>ORECC</v>
-      </c>
-    </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A9" t="str" cm="1">
-        <f t="array" ref="A9:A31">TRANSPOSE(A1:W1)</f>
-        <v>001  ORECC</v>
-      </c>
-      <c r="C9" t="str" cm="1">
-        <f t="array" ref="C9:E9">_xlfn.TEXTSPLIT(A9," ")</f>
-        <v>001</v>
-      </c>
-      <c r="D9" t="str">
-        <v/>
-      </c>
-      <c r="E9" t="str">
-        <v>ORECC</v>
-      </c>
-    </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A10" t="str">
-        <v>002 TROFIE</v>
-      </c>
-      <c r="C10" t="str" cm="1">
-        <f t="array" ref="C10:D10">_xlfn.TEXTSPLIT(A10," ")</f>
-        <v>002</v>
-      </c>
-      <c r="D10" t="str">
-        <v>TROFIE</v>
-      </c>
-    </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A11" t="str">
-        <v>003 MACCH.</v>
-      </c>
-      <c r="C11" t="str" cm="1">
-        <f t="array" ref="C11:D11">_xlfn.TEXTSPLIT(A11," ")</f>
-        <v>003</v>
-      </c>
-      <c r="D11" t="str">
-        <v>MACCH.</v>
-      </c>
-    </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A12" t="str">
-        <v>004 CAVAT.</v>
-      </c>
-      <c r="C12" t="str" cm="1">
-        <f t="array" ref="C12:D12">_xlfn.TEXTSPLIT(A12," ")</f>
-        <v>004</v>
-      </c>
-      <c r="D12" t="str">
-        <v>CAVAT.</v>
-      </c>
-    </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A13" t="str">
-        <v>005  OREC_INT</v>
-      </c>
-      <c r="C13" t="str" cm="1">
-        <f t="array" ref="C13:E13">_xlfn.TEXTSPLIT(A13," ")</f>
-        <v>005</v>
-      </c>
-      <c r="D13" t="str">
-        <v/>
-      </c>
-      <c r="E13" t="str">
-        <v>OREC_INT</v>
-      </c>
-    </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A14" t="str">
-        <v>006 MACC_INT</v>
-      </c>
-      <c r="C14" t="str" cm="1">
-        <f t="array" ref="C14:D14">_xlfn.TEXTSPLIT(A14," ")</f>
-        <v>006</v>
-      </c>
-      <c r="D14" t="str">
-        <v>MACC_INT</v>
-      </c>
-    </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A15" t="str">
-        <v>007  MAR.INT</v>
-      </c>
-      <c r="C15" t="str" cm="1">
-        <f t="array" ref="C15:E15">_xlfn.TEXTSPLIT(A15," ")</f>
-        <v>007</v>
-      </c>
-      <c r="D15" t="str">
-        <v/>
-      </c>
-      <c r="E15" t="str">
-        <v>MAR.INT</v>
-      </c>
-    </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A16" t="str">
-        <v>008 cav. Int</v>
-      </c>
-      <c r="C16" t="str" cm="1">
-        <f t="array" ref="C16:E16">_xlfn.TEXTSPLIT(A16," ")</f>
-        <v>008</v>
-      </c>
-      <c r="D16" t="str">
-        <v>cav.</v>
-      </c>
-      <c r="E16" t="str">
-        <v>Int</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" t="str">
-        <v>009  MARIT.</v>
-      </c>
-      <c r="C17" t="str" cm="1">
-        <f t="array" ref="C17:E17">_xlfn.TEXTSPLIT(A17," ")</f>
-        <v>009</v>
-      </c>
-      <c r="D17" t="str">
-        <v/>
-      </c>
-      <c r="E17" t="str">
-        <v>MARIT.</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" t="str">
-        <v>010  TROCC</v>
-      </c>
-      <c r="C18" t="str" cm="1">
-        <f t="array" ref="C18:E18">_xlfn.TEXTSPLIT(A18," ")</f>
-        <v>010</v>
-      </c>
-      <c r="D18" t="str">
-        <v/>
-      </c>
-      <c r="E18" t="str">
-        <v>TROCC</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" t="str">
-        <v>011  STRASC</v>
-      </c>
-      <c r="C19" t="str" cm="1">
-        <f t="array" ref="C19:E19">_xlfn.TEXTSPLIT(A19," ")</f>
-        <v>011</v>
-      </c>
-      <c r="D19" t="str">
-        <v/>
-      </c>
-      <c r="E19" t="str">
-        <v>STRASC</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" t="str">
-        <v>027 ORECCHIETTE_C.RAPA</v>
-      </c>
-      <c r="C20" t="str" cm="1">
-        <f t="array" ref="C20:D20">_xlfn.TEXTSPLIT(A20," ")</f>
-        <v>027</v>
-      </c>
-      <c r="D20" t="str">
-        <v>ORECCHIETTE_C.RAPA</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" t="str">
-        <v>030   ORECCHIETTE_SECCHE</v>
-      </c>
-      <c r="C21" t="str" cm="1">
-        <f t="array" ref="C21:F21">_xlfn.TEXTSPLIT(A21," ")</f>
-        <v>030</v>
-      </c>
-      <c r="D21" t="str">
-        <v/>
-      </c>
-      <c r="E21" t="str">
-        <v/>
-      </c>
-      <c r="F21" t="str">
-        <v>ORECCHIETTE_SECCHE</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" t="str">
-        <v>032   CAVATELLI_SECCHE</v>
-      </c>
-      <c r="C22" t="str" cm="1">
-        <f t="array" ref="C22:F22">_xlfn.TEXTSPLIT(A22," ")</f>
-        <v>032</v>
-      </c>
-      <c r="D22" t="str">
-        <v/>
-      </c>
-      <c r="E22" t="str">
-        <v/>
-      </c>
-      <c r="F22" t="str">
-        <v>CAVATELLI_SECCHE</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" t="str">
-        <v>034   TROCCOLI_SECCHE</v>
-      </c>
-      <c r="C23" t="str" cm="1">
-        <f t="array" ref="C23:F23">_xlfn.TEXTSPLIT(A23," ")</f>
-        <v>034</v>
-      </c>
-      <c r="D23" t="str">
-        <v/>
-      </c>
-      <c r="E23" t="str">
-        <v/>
-      </c>
-      <c r="F23" t="str">
-        <v>TROCCOLI_SECCHE</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" t="str">
-        <v>035 PAPP_SEMOLA_SECCHE</v>
-      </c>
-      <c r="C24" t="str" cm="1">
-        <f t="array" ref="C24:D24">_xlfn.TEXTSPLIT(A24," ")</f>
-        <v>035</v>
-      </c>
-      <c r="D24" t="str">
-        <v>PAPP_SEMOLA_SECCHE</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" t="str">
-        <v>036 TAGLIATELLE_SEMOLA_SECCHE</v>
-      </c>
-      <c r="C25" t="str" cm="1">
-        <f t="array" ref="C25:D25">_xlfn.TEXTSPLIT(A25," ")</f>
-        <v>036</v>
-      </c>
-      <c r="D25" t="str">
-        <v>TAGLIATELLE_SEMOLA_SECCHE</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" t="str">
-        <v>39 MARITATI_INT_SECCHE</v>
-      </c>
-      <c r="C26" t="str" cm="1">
-        <f t="array" ref="C26:D26">_xlfn.TEXTSPLIT(A26," ")</f>
-        <v>39</v>
-      </c>
-      <c r="D26" t="str">
-        <v>MARITATI_INT_SECCHE</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" t="str">
-        <v>042   PAPP_UOVO_SECCHE</v>
-      </c>
-      <c r="C27" t="str" cm="1">
-        <f t="array" ref="C27:F27">_xlfn.TEXTSPLIT(A27," ")</f>
-        <v>042</v>
-      </c>
-      <c r="D27" t="str">
-        <v/>
-      </c>
-      <c r="E27" t="str">
-        <v/>
-      </c>
-      <c r="F27" t="str">
-        <v>PAPP_UOVO_SECCHE</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" t="str">
-        <v>04 orecch.int_SECCHE</v>
-      </c>
-      <c r="C28" t="str" cm="1">
-        <f t="array" ref="C28:D28">_xlfn.TEXTSPLIT(A28," ")</f>
-        <v>04</v>
-      </c>
-      <c r="D28" t="str">
-        <v>orecch.int_SECCHE</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" t="str">
-        <v>0026 ORECCHIETTE_ARSO_SECCHE</v>
-      </c>
-      <c r="C29" t="str" cm="1">
-        <f t="array" ref="C29:D29">_xlfn.TEXTSPLIT(A29," ")</f>
-        <v>0026</v>
-      </c>
-      <c r="D29" t="str">
-        <v>ORECCHIETTE_ARSO_SECCHE</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" t="str">
-        <v>124     FUSILLI</v>
-      </c>
-      <c r="C30" t="str" cm="1">
-        <f t="array" ref="C30:H30">_xlfn.TEXTSPLIT(A30," ")</f>
-        <v>124</v>
-      </c>
-      <c r="D30" t="str">
-        <v/>
-      </c>
-      <c r="E30" t="str">
-        <v/>
-      </c>
-      <c r="F30" t="str">
-        <v/>
-      </c>
-      <c r="G30" t="str">
-        <v/>
-      </c>
-      <c r="H30" t="str">
-        <v>FUSILLI</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" t="str">
-        <v>125     FUSILLI_INT</v>
-      </c>
-      <c r="C31" t="str" cm="1">
-        <f t="array" ref="C31:H31">_xlfn.TEXTSPLIT(A31," ")</f>
-        <v>125</v>
-      </c>
-      <c r="D31" t="str">
-        <v/>
-      </c>
-      <c r="E31" t="str">
-        <v/>
-      </c>
-      <c r="F31" t="str">
-        <v/>
-      </c>
-      <c r="G31" t="str">
-        <v/>
-      </c>
-      <c r="H31" t="str">
-        <v>FUSILLI_INT</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1342C7CE-6C97-4939-8FDB-08E523DE384D}">
   <dimension ref="A1:M18"/>
   <sheetViews>
@@ -36724,28 +36216,28 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C1" t="s">
         <v>79</v>
       </c>
-      <c r="B1" t="s">
-        <v>77</v>
-      </c>
-      <c r="C1" t="s">
-        <v>81</v>
-      </c>
       <c r="D1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E1" t="s">
+        <v>74</v>
+      </c>
+      <c r="F1" t="s">
         <v>78</v>
       </c>
-      <c r="E1" t="s">
-        <v>76</v>
-      </c>
-      <c r="F1" t="s">
-        <v>80</v>
-      </c>
       <c r="G1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="H1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -36753,10 +36245,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -36779,10 +36271,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E3" s="149">
         <v>5</v>
@@ -36802,13 +36294,13 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C4" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D4" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E4" s="149">
         <v>6</v>
@@ -36823,7 +36315,7 @@
         <v>1</v>
       </c>
       <c r="J4" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="K4">
         <f>COLUMN(Tabella1[[#Headers],[Valore]])</f>
@@ -36835,13 +36327,13 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C5" t="s">
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E5" s="149">
         <v>6</v>
@@ -36856,7 +36348,7 @@
         <v>1</v>
       </c>
       <c r="J5" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="K5">
         <f>COLUMN(Tabella1[[#Headers],[Lunghezza]])</f>
@@ -36868,10 +36360,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C6" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E6" s="149">
         <v>6</v>
@@ -36886,7 +36378,7 @@
         <v>0</v>
       </c>
       <c r="J6" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="K6">
         <f>COLUMN(Tabella1[[#Headers],[default]])</f>
@@ -36898,7 +36390,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C7" t="s">
         <v>1</v>
@@ -36921,13 +36413,13 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C8" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D8" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="E8" s="149">
         <v>15</v>
@@ -36947,13 +36439,13 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C9" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D9" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E9" s="149">
         <v>1</v>
@@ -36973,13 +36465,13 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C10" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D10" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E10" s="149">
         <v>15</v>
@@ -36999,10 +36491,10 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C11" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E11" s="149">
         <v>15</v>
@@ -37022,13 +36514,13 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C12" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D12" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E12" s="149">
         <v>15</v>
@@ -37048,10 +36540,10 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C13" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D13">
         <v>1</v>
@@ -37074,13 +36566,13 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C14" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D14" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E14" s="149">
         <v>1</v>
@@ -37203,7 +36695,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B16287B-BE6D-4D6F-A3D6-60EFDE11C93B}">
   <dimension ref="A1:AA32"/>
   <sheetViews>
@@ -37227,25 +36719,25 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C1" t="s">
         <v>79</v>
       </c>
-      <c r="B1" t="s">
-        <v>77</v>
-      </c>
-      <c r="C1" t="s">
-        <v>81</v>
-      </c>
       <c r="D1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E1" t="s">
+        <v>74</v>
+      </c>
+      <c r="F1" t="s">
         <v>78</v>
       </c>
-      <c r="E1" t="s">
-        <v>76</v>
-      </c>
-      <c r="F1" t="s">
-        <v>80</v>
-      </c>
       <c r="G1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -37253,10 +36745,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E2" s="149">
         <v>2</v>
@@ -37273,10 +36765,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E3" s="149">
         <v>5</v>
@@ -37293,10 +36785,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C4" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E4" s="149">
         <v>15</v>
@@ -37313,10 +36805,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C5" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E5" s="149">
         <v>30</v>
@@ -37333,10 +36825,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C6" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E6" s="149">
         <v>2</v>
@@ -37353,10 +36845,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C7" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E7" s="149">
         <v>7</v>
@@ -37373,10 +36865,10 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C8" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E8" s="149">
         <v>9</v>
@@ -37393,10 +36885,10 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C9" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E9" s="149">
         <v>9</v>
@@ -37413,10 +36905,10 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C10" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E10" s="149">
         <v>4</v>
@@ -37433,10 +36925,10 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C11" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E11" s="149">
         <v>1</v>
@@ -37453,10 +36945,10 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C12" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E12" s="149">
         <v>2</v>
@@ -37473,10 +36965,10 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C13" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E13" s="149">
         <v>1</v>
@@ -37493,10 +36985,10 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C14" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E14" s="149">
         <v>1</v>
@@ -37513,10 +37005,10 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C15" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E15">
         <v>6</v>
@@ -37533,10 +37025,10 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C16" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E16">
         <v>2</v>
@@ -37553,10 +37045,10 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C17" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E17">
         <v>1</v>
@@ -37573,10 +37065,10 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C18" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E18">
         <v>1</v>
@@ -37593,10 +37085,10 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C19" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E19">
         <v>1</v>
@@ -37613,10 +37105,10 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C20" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E20">
         <v>5</v>
@@ -37633,10 +37125,10 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C21" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E21">
         <v>1</v>
@@ -37653,10 +37145,10 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C22" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E22" s="149">
         <v>1</v>
@@ -37673,7 +37165,7 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="E23">
         <v>7</v>
@@ -37687,7 +37179,7 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E24">
         <v>3</v>
@@ -37701,7 +37193,7 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C25" t="s">
         <v>1</v>
@@ -37721,7 +37213,7 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="E26">
         <v>6</v>
@@ -37735,7 +37227,7 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E27">
         <v>9</v>
@@ -37749,10 +37241,10 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C28" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E28" s="149">
         <v>23</v>
@@ -37853,7 +37345,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F79B6B3F-A53A-40B4-A159-5A53FC02F8ED}">
   <dimension ref="A1:O20"/>
   <sheetViews>
@@ -37877,22 +37369,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C1" t="s">
         <v>79</v>
       </c>
-      <c r="B1" t="s">
-        <v>77</v>
-      </c>
-      <c r="C1" t="s">
-        <v>81</v>
-      </c>
       <c r="D1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E1" t="s">
+        <v>74</v>
+      </c>
+      <c r="F1" t="s">
         <v>78</v>
-      </c>
-      <c r="E1" t="s">
-        <v>76</v>
-      </c>
-      <c r="F1" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -37900,10 +37392,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E2" s="149">
         <v>2</v>
@@ -37917,10 +37409,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E3" s="149">
         <v>5</v>
@@ -37934,10 +37426,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C4" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E4" s="149">
         <v>15</v>
@@ -37951,10 +37443,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C5" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E5" s="149">
         <v>30</v>
@@ -37968,10 +37460,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C6" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E6" s="149">
         <v>2</v>
@@ -37985,10 +37477,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C7" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E7" s="149">
         <v>7</v>
@@ -38002,10 +37494,10 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C8" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E8" s="149">
         <v>9</v>
@@ -38019,10 +37511,10 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C9" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E9" s="149">
         <v>9</v>
@@ -38036,10 +37528,10 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C10" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E10" s="149">
         <v>1</v>
@@ -38053,10 +37545,10 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C11" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E11" s="149">
         <v>2</v>
@@ -38070,10 +37562,10 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C12" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E12" s="149">
         <v>1</v>
@@ -38087,10 +37579,10 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C13" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E13" s="149">
         <v>1</v>
@@ -38104,10 +37596,10 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C14" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E14" s="149">
         <v>1</v>
@@ -38121,7 +37613,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C15" t="s">
         <v>1</v>
@@ -38138,10 +37630,10 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C16" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E16" s="149">
         <v>23</v>
@@ -38203,15 +37695,18 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BA3FAC6-9F99-4F57-A723-973EE87B9D46}">
   <dimension ref="A1:A32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+      <selection activeCell="B1" sqref="B1:B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="27.140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="83" t="s">
@@ -38300,22 +37795,22 @@
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="84" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="84" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="83" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="21" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="131" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="22" spans="1:1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -38325,7 +37820,7 @@
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="82" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
@@ -38355,22 +37850,22 @@
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" s="81" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" s="81" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" s="81" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" s="81" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -38378,12 +37873,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FDE1613-D14A-4CEE-86E0-5B12B3154235}">
-  <dimension ref="A1:I18"/>
+  <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+      <selection activeCell="D2" sqref="D2:D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -38394,38 +37889,38 @@
     <col min="5" max="5" width="9.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="155" t="s">
-        <v>113</v>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="153" t="s">
+        <v>111</v>
       </c>
       <c r="B1" s="150" t="s">
+        <v>159</v>
+      </c>
+      <c r="C1" s="160" t="s">
+        <v>160</v>
+      </c>
+      <c r="D1" s="150" t="s">
+        <v>161</v>
+      </c>
+      <c r="E1" s="150" t="s">
+        <v>185</v>
+      </c>
+      <c r="F1" s="150" t="s">
+        <v>162</v>
+      </c>
+      <c r="G1" s="150" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="157" t="s">
+        <v>164</v>
+      </c>
+      <c r="B2" s="151" t="s">
+        <v>139</v>
+      </c>
+      <c r="C2" t="s">
         <v>178</v>
-      </c>
-      <c r="C1" s="156" t="s">
-        <v>179</v>
-      </c>
-      <c r="D1" s="150" t="s">
-        <v>180</v>
-      </c>
-      <c r="E1" s="150" t="s">
-        <v>181</v>
-      </c>
-      <c r="F1" s="150" t="s">
-        <v>182</v>
-      </c>
-      <c r="G1" s="150" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="154" t="s">
-        <v>184</v>
-      </c>
-      <c r="B2" s="151" t="s">
-        <v>155</v>
-      </c>
-      <c r="C2" t="s">
-        <v>199</v>
       </c>
       <c r="D2" s="150">
         <v>500</v>
@@ -38438,15 +37933,15 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>185</v>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="151" t="s">
+        <v>165</v>
       </c>
       <c r="B3" s="151" t="s">
-        <v>156</v>
+        <v>140</v>
       </c>
       <c r="C3" t="s">
-        <v>200</v>
+        <v>179</v>
       </c>
       <c r="D3" s="150">
         <v>500</v>
@@ -38459,15 +37954,15 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="154" t="s">
-        <v>186</v>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="157" t="s">
+        <v>166</v>
       </c>
       <c r="B4" s="151" t="s">
-        <v>156</v>
+        <v>140</v>
       </c>
       <c r="C4" t="s">
-        <v>201</v>
+        <v>180</v>
       </c>
       <c r="D4" s="150">
         <v>500</v>
@@ -38480,15 +37975,15 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>187</v>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="151" t="s">
+        <v>184</v>
       </c>
       <c r="B5" s="151" t="s">
-        <v>157</v>
+        <v>141</v>
       </c>
       <c r="C5" t="s">
-        <v>202</v>
+        <v>181</v>
       </c>
       <c r="D5" s="150">
         <v>500</v>
@@ -38501,15 +37996,15 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="154" t="s">
-        <v>188</v>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="157" t="s">
+        <v>167</v>
       </c>
       <c r="B6" s="151" t="s">
-        <v>158</v>
+        <v>142</v>
       </c>
       <c r="C6" t="s">
-        <v>159</v>
+        <v>143</v>
       </c>
       <c r="D6" s="150">
         <v>350</v>
@@ -38522,15 +38017,15 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>189</v>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="151" t="s">
+        <v>168</v>
       </c>
       <c r="B7" s="151" t="s">
-        <v>160</v>
+        <v>144</v>
       </c>
       <c r="C7" t="s">
-        <v>161</v>
+        <v>145</v>
       </c>
       <c r="D7" s="150">
         <v>350</v>
@@ -38543,15 +38038,15 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="154" t="s">
-        <v>190</v>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="157" t="s">
+        <v>169</v>
       </c>
       <c r="B8" s="151" t="s">
-        <v>162</v>
+        <v>146</v>
       </c>
       <c r="C8" t="s">
-        <v>203</v>
+        <v>182</v>
       </c>
       <c r="D8" s="150">
         <v>350</v>
@@ -38564,15 +38059,15 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>191</v>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="151" t="s">
+        <v>170</v>
       </c>
       <c r="B9" s="151" t="s">
-        <v>163</v>
+        <v>147</v>
       </c>
       <c r="C9" t="s">
-        <v>164</v>
+        <v>186</v>
       </c>
       <c r="D9" s="150">
         <v>350</v>
@@ -38584,16 +38079,17 @@
       <c r="G9" s="150">
         <v>4</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="154" t="s">
-        <v>192</v>
+      <c r="H9" s="159"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="157" t="s">
+        <v>171</v>
       </c>
       <c r="B10" s="151" t="s">
-        <v>165</v>
-      </c>
-      <c r="C10" t="s">
-        <v>166</v>
+        <v>148</v>
+      </c>
+      <c r="C10" s="156" t="s">
+        <v>187</v>
       </c>
       <c r="D10" s="150">
         <v>350</v>
@@ -38606,15 +38102,15 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>193</v>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="151" t="s">
+        <v>172</v>
       </c>
       <c r="B11" s="151" t="s">
-        <v>167</v>
+        <v>149</v>
       </c>
       <c r="C11" t="s">
-        <v>168</v>
+        <v>188</v>
       </c>
       <c r="D11" s="150">
         <v>350</v>
@@ -38627,15 +38123,15 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="154" t="s">
-        <v>194</v>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="157" t="s">
+        <v>173</v>
       </c>
       <c r="B12" s="151" t="s">
-        <v>169</v>
+        <v>150</v>
       </c>
       <c r="C12" t="s">
-        <v>170</v>
+        <v>151</v>
       </c>
       <c r="D12" s="150">
         <v>350</v>
@@ -38648,15 +38144,15 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>195</v>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="151" t="s">
+        <v>174</v>
       </c>
       <c r="B13" s="151" t="s">
-        <v>171</v>
+        <v>152</v>
       </c>
       <c r="C13" t="s">
-        <v>172</v>
+        <v>153</v>
       </c>
       <c r="D13" s="150">
         <v>350</v>
@@ -38669,15 +38165,15 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="154" t="s">
-        <v>196</v>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="157" t="s">
+        <v>175</v>
       </c>
       <c r="B14" s="151" t="s">
-        <v>173</v>
+        <v>154</v>
       </c>
       <c r="C14" t="s">
-        <v>174</v>
+        <v>155</v>
       </c>
       <c r="D14" s="150">
         <v>350</v>
@@ -38690,15 +38186,15 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>197</v>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="151" t="s">
+        <v>176</v>
       </c>
       <c r="B15" s="151" t="s">
-        <v>175</v>
+        <v>156</v>
       </c>
       <c r="C15" t="s">
-        <v>176</v>
+        <v>157</v>
       </c>
       <c r="D15" s="150">
         <v>250</v>
@@ -38713,15 +38209,15 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="153" t="s">
-        <v>198</v>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="158" t="s">
+        <v>177</v>
       </c>
       <c r="B16" s="151" t="s">
-        <v>177</v>
+        <v>158</v>
       </c>
       <c r="C16" t="s">
-        <v>204</v>
+        <v>183</v>
       </c>
       <c r="D16" s="150">
         <v>250</v>
@@ -38736,11 +38232,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I18" s="159"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="A2:B16" numberStoredAsText="1"/>
+  </ignoredErrors>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>

</xml_diff>